<commit_message>
Added new histograms and updated analysis with new control cut-offs
</commit_message>
<xml_diff>
--- a/Results/UVC_CPD_percentage_old skin_V2.xlsx
+++ b/Results/UVC_CPD_percentage_old skin_V2.xlsx
@@ -1,80 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MBender\Arbeit\Github\EKB\BFS_UVC\Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58EC74F-2C72-4011-90C1-CE1130489E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>comparison</t>
-  </si>
-  <si>
-    <t>diff</t>
-  </si>
-  <si>
-    <t>lwr.ci</t>
-  </si>
-  <si>
-    <t>upr.ci</t>
-  </si>
-  <si>
-    <t>pval</t>
-  </si>
-  <si>
-    <t>pval.adj</t>
-  </si>
-  <si>
-    <t>222nm Basal</t>
-  </si>
-  <si>
-    <t>30 J/m²-Control</t>
-  </si>
-  <si>
-    <t>300 J/m²-Control</t>
-  </si>
-  <si>
-    <t>1000 J/m²-Control</t>
-  </si>
-  <si>
-    <t>2000 J/m²-Control</t>
-  </si>
-  <si>
-    <t>222nm Suprabasal</t>
-  </si>
-  <si>
-    <t>254nm Basal</t>
-  </si>
-  <si>
-    <t>254nm Suprabasal</t>
-  </si>
-  <si>
-    <t>Erklärung: siehe young skin</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lwr.ci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upr.ci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pval.adj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">222nm Basal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 J/m²-Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 J/m²-Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000 J/m²-Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000 J/m²-Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">222nm Suprabasal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254nm Basal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254nm Suprabasal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -83,18 +73,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,23 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -407,19 +381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,380 +411,376 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>-0.145454545454545</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>-0.170574416354483</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>-0.120334674554608</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>-0.145454545454545</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>-0.170574416354483</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>-0.120334674554608</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>-0.145454545454545</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>-0.170574416354483</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>-0.120334674554608</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>-0.145454545454545</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>-0.170574416354483</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>-0.120334674554608</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>0.381818181818182</v>
       </c>
-      <c r="D6">
-        <v>-1.1877349276896001</v>
-      </c>
-      <c r="E6">
+      <c r="D6" t="n">
+        <v>-1.1877349276896</v>
+      </c>
+      <c r="E6" t="n">
         <v>1.95137129132596</v>
       </c>
-      <c r="F6">
-        <v>0.92862698138091104</v>
-      </c>
-      <c r="G6">
-        <v>0.99618030414143599</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F6" t="n">
+        <v>0.928635992870718</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.996181383660215</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>0.236363636363636</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>-1.33318947314415</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>1.80591674587142</v>
       </c>
-      <c r="F7">
-        <v>0.98664569545168102</v>
-      </c>
-      <c r="G7">
-        <v>0.99618030414143599</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F7" t="n">
+        <v>0.98664752039273</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.996181383660215</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>1.02727272727273</v>
       </c>
-      <c r="D8">
-        <v>-0.54228038223505504</v>
-      </c>
-      <c r="E8">
-        <v>2.5968258367805102</v>
-      </c>
-      <c r="F8">
-        <v>0.29651809755616199</v>
-      </c>
-      <c r="G8">
-        <v>0.43129905099078197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D8" t="n">
+        <v>-0.542280382235055</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.59682583678051</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.296631455016251</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.431463934569092</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>1.82727272727273</v>
       </c>
-      <c r="D9">
-        <v>0.25771961776494501</v>
-      </c>
-      <c r="E9">
+      <c r="D9" t="n">
+        <v>0.257719617764945</v>
+      </c>
+      <c r="E9" t="n">
         <v>3.39682583678051</v>
       </c>
-      <c r="F9">
-        <v>1.75852076880153E-2</v>
-      </c>
-      <c r="G9">
-        <v>2.8136332300824501E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F9" t="n">
+        <v>0.0176751386356047</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0282802218169675</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
-        <v>2.3181818181818201</v>
-      </c>
-      <c r="D10">
-        <v>-19.143931678382099</v>
-      </c>
-      <c r="E10">
+      <c r="C10" t="n">
+        <v>2.31818181818182</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-19.1439316783821</v>
+      </c>
+      <c r="E10" t="n">
         <v>23.7802953147457</v>
       </c>
-      <c r="F10">
-        <v>0.99618030414143599</v>
-      </c>
-      <c r="G10">
-        <v>0.99618030414143599</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F10" t="n">
+        <v>0.996181383660215</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.996181383660215</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>7.3</v>
       </c>
-      <c r="D11">
-        <v>-14.162113496563901</v>
-      </c>
-      <c r="E11">
-        <v>28.762113496563899</v>
-      </c>
-      <c r="F11">
-        <v>0.80531849165541403</v>
-      </c>
-      <c r="G11">
-        <v>0.99116122049897104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D11" t="n">
+        <v>-14.1621134965639</v>
+      </c>
+      <c r="E11" t="n">
+        <v>28.7621134965639</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.80526985717399</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.99110136267568</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>30.5818181818182</v>
       </c>
-      <c r="D12">
-        <v>9.1197046852542893</v>
-      </c>
-      <c r="E12">
-        <v>52.043931678382101</v>
-      </c>
-      <c r="F12">
-        <v>2.7613317834080898E-3</v>
-      </c>
-      <c r="G12">
-        <v>4.9090342816143903E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D12" t="n">
+        <v>9.11970468525429</v>
+      </c>
+      <c r="E12" t="n">
+        <v>52.0439316783821</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0027113400056048</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.00482016000996409</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
-        <v>45.809090909090898</v>
-      </c>
-      <c r="D13">
+      <c r="C13" t="n">
+        <v>45.8090909090909</v>
+      </c>
+      <c r="D13" t="n">
         <v>24.346977412527</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>67.2712044056548</v>
       </c>
-      <c r="F13">
-        <v>8.4036539405030197E-6</v>
-      </c>
-      <c r="G13">
-        <v>1.9208351864006901E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F13" t="n">
+        <v>0.00000669717784762547</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0000153078350802868</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>10.8909090909091</v>
       </c>
-      <c r="D14">
-        <v>-9.6917179725868792</v>
-      </c>
-      <c r="E14">
+      <c r="D14" t="n">
+        <v>-9.69171797258688</v>
+      </c>
+      <c r="E14" t="n">
         <v>31.4735361544051</v>
       </c>
-      <c r="F14">
-        <v>0.48105545039924202</v>
-      </c>
-      <c r="G14">
-        <v>0.641407267198989</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F14" t="n">
+        <v>0.481171924633132</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.64156256617751</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15">
-        <v>35.563636363636398</v>
-      </c>
-      <c r="D15">
+      <c r="C15" t="n">
+        <v>35.5636363636364</v>
+      </c>
+      <c r="D15" t="n">
         <v>14.9810093001404</v>
       </c>
-      <c r="E15">
-        <v>56.146263427132297</v>
-      </c>
-      <c r="F15">
-        <v>2.5310720330706799E-4</v>
-      </c>
-      <c r="G15">
-        <v>5.0621440661413597E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E15" t="n">
+        <v>56.1462634271323</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.000219960111104478</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.000439920222208956</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C16">
-        <v>66.390909090909105</v>
-      </c>
-      <c r="D16">
+      <c r="C16" t="n">
+        <v>66.3909090909091</v>
+      </c>
+      <c r="D16" t="n">
         <v>45.8082820274131</v>
       </c>
-      <c r="E16">
-        <v>86.973536154405096</v>
-      </c>
-      <c r="F16">
-        <v>1.01391783857707E-10</v>
-      </c>
-      <c r="G16">
-        <v>2.70378090287219E-10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E16" t="n">
+        <v>86.9735361544051</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0000000000861011262287548</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.000000000229603003276679</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17">
-        <v>67.209090909090904</v>
-      </c>
-      <c r="D17">
-        <v>46.626463845594898</v>
-      </c>
-      <c r="E17">
-        <v>87.791717972586895</v>
-      </c>
-      <c r="F17">
-        <v>7.7694961575502904E-11</v>
-      </c>
-      <c r="G17">
-        <v>2.4862387704160899E-10</v>
+      <c r="C17" t="n">
+        <v>67.2090909090909</v>
+      </c>
+      <c r="D17" t="n">
+        <v>46.6264638455949</v>
+      </c>
+      <c r="E17" t="n">
+        <v>87.7917179725869</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0000000000830741031521143</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.000000000229603003276679</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ran analysis with new .csv files
</commit_message>
<xml_diff>
--- a/Results/UVC_CPD_percentage_old skin_V2.xlsx
+++ b/Results/UVC_CPD_percentage_old skin_V2.xlsx
@@ -419,19 +419,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.145454545454545</v>
+        <v>0.390909090909091</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.170574416354483</v>
+        <v>-1.33267531145035</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.120334674554608</v>
+        <v>2.11449349326853</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.943287606242385</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.99996960525172</v>
       </c>
     </row>
     <row r="3">
@@ -442,19 +442,19 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.145454545454545</v>
+        <v>0.254545454545455</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.170574416354483</v>
+        <v>-1.46903894781399</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.120334674554608</v>
+        <v>1.9781298569049</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.987571732951626</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.99996960525172</v>
       </c>
     </row>
     <row r="4">
@@ -465,19 +465,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.145454545454545</v>
+        <v>0.0545454545454545</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.170574416354483</v>
+        <v>-1.66903894781399</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.120334674554608</v>
+        <v>1.7781298569049</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.99996960525172</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.99996960525172</v>
       </c>
     </row>
     <row r="5">
@@ -488,19 +488,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.145454545454545</v>
+        <v>1.41818181818182</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.170574416354483</v>
+        <v>-0.305402584177623</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.120334674554608</v>
+        <v>3.14176622054126</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.134397398839095</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.30719405448936</v>
       </c>
     </row>
     <row r="6">
@@ -520,10 +520,10 @@
         <v>1.95137129132596</v>
       </c>
       <c r="F6" t="n">
-        <v>0.928635992870718</v>
+        <v>0.928618001972295</v>
       </c>
       <c r="G6" t="n">
-        <v>0.996181383660215</v>
+        <v>0.99996960525172</v>
       </c>
     </row>
     <row r="7">
@@ -543,10 +543,10 @@
         <v>1.80591674587142</v>
       </c>
       <c r="F7" t="n">
-        <v>0.98664752039273</v>
+        <v>0.986643604872859</v>
       </c>
       <c r="G7" t="n">
-        <v>0.996181383660215</v>
+        <v>0.99996960525172</v>
       </c>
     </row>
     <row r="8">
@@ -566,10 +566,10 @@
         <v>2.59682583678051</v>
       </c>
       <c r="F8" t="n">
-        <v>0.296631455016251</v>
+        <v>0.2965222266076</v>
       </c>
       <c r="G8" t="n">
-        <v>0.431463934569092</v>
+        <v>0.593044453215201</v>
       </c>
     </row>
     <row r="9">
@@ -589,10 +589,10 @@
         <v>3.39682583678051</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0176751386356047</v>
+        <v>0.0176058844871828</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0282802218169675</v>
+        <v>0.0469490252991542</v>
       </c>
     </row>
     <row r="10">
@@ -612,10 +612,10 @@
         <v>23.7802953147457</v>
       </c>
       <c r="F10" t="n">
-        <v>0.996181383660215</v>
+        <v>0.996181161513232</v>
       </c>
       <c r="G10" t="n">
-        <v>0.996181383660215</v>
+        <v>0.99996960525172</v>
       </c>
     </row>
     <row r="11">
@@ -635,10 +635,10 @@
         <v>28.7621134965639</v>
       </c>
       <c r="F11" t="n">
-        <v>0.80526985717399</v>
+        <v>0.805279658652863</v>
       </c>
       <c r="G11" t="n">
-        <v>0.99110136267568</v>
+        <v>0.99996960525172</v>
       </c>
     </row>
     <row r="12">
@@ -658,10 +658,10 @@
         <v>52.0439316783821</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0027113400056048</v>
+        <v>0.00276156704646191</v>
       </c>
       <c r="G12" t="n">
-        <v>0.00482016000996409</v>
+        <v>0.00883701454867811</v>
       </c>
     </row>
     <row r="13">
@@ -681,10 +681,10 @@
         <v>67.2712044056548</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00000669717784762547</v>
+        <v>0.00000451606832641005</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0000153078350802868</v>
+        <v>0.0000240856977408536</v>
       </c>
     </row>
     <row r="14">
@@ -704,10 +704,10 @@
         <v>31.4735361544051</v>
       </c>
       <c r="F14" t="n">
-        <v>0.481171924633132</v>
+        <v>0.481124324802707</v>
       </c>
       <c r="G14" t="n">
-        <v>0.64156256617751</v>
+        <v>0.85533213298259</v>
       </c>
     </row>
     <row r="15">
@@ -727,10 +727,10 @@
         <v>56.1462634271323</v>
       </c>
       <c r="F15" t="n">
-        <v>0.000219960111104478</v>
+        <v>0.000246981671981783</v>
       </c>
       <c r="G15" t="n">
-        <v>0.000439920222208956</v>
+        <v>0.000987926687927132</v>
       </c>
     </row>
     <row r="16">
@@ -750,10 +750,10 @@
         <v>86.9735361544051</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0000000000861011262287548</v>
+        <v>0.0000000000982907089053242</v>
       </c>
       <c r="G16" t="n">
-        <v>0.000000000229603003276679</v>
+        <v>0.00000000141969280775811</v>
       </c>
     </row>
     <row r="17">
@@ -773,10 +773,10 @@
         <v>87.7917179725869</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0000000000830741031521143</v>
+        <v>0.000000000177461600969764</v>
       </c>
       <c r="G17" t="n">
-        <v>0.000000000229603003276679</v>
+        <v>0.00000000141969280775811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>